<commit_message>
Adding to MetaData file and some other minor changes
</commit_message>
<xml_diff>
--- a/Data/0.MetaData.xlsx
+++ b/Data/0.MetaData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asaf Bernstein\Dropbox (MIT)\RatingAgenciesFileStructureTest\LocalRepositories\AB\Introduction-Rating-Agencies\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Introduction-Rating-Agencies\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="6924" tabRatio="929"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="6930" tabRatio="929" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="Moodys_1909_Bond_Ratings" sheetId="8" r:id="rId8"/>
     <sheet name="HoldingsData_Final_wIndustry" sheetId="2" r:id="rId9"/>
     <sheet name="Bid_Ask_1908_1909_Combined" sheetId="3" r:id="rId10"/>
+    <sheet name="city_state_list" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="660">
   <si>
     <t>Moodys_1909_Stock_Ratings</t>
   </si>
@@ -1989,6 +1990,30 @@
   </si>
   <si>
     <t>intraday_data_cleaned_v1.dta</t>
+  </si>
+  <si>
+    <t>city_state_list</t>
+  </si>
+  <si>
+    <t>Lists all investor state &amp; city in holdings data</t>
+  </si>
+  <si>
+    <t>std_name</t>
+  </si>
+  <si>
+    <t>Lists all cleaned up investor state &amp; city in holdings data from variavle "investor_city_temp" &amp; "investor_state_temp" variable in HoldingsData_Final_wIndustry.dta</t>
+  </si>
+  <si>
+    <t>city_state_list.dta</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>taging the geographic type: state/city &amp; foreign/domestic</t>
+  </si>
+  <si>
+    <t>geographic names, including both city and state</t>
   </si>
 </sst>
 </file>
@@ -2118,13 +2143,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2440,30 +2465,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L12"/>
+  <dimension ref="B1:L13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.21875" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
-    <col min="6" max="6" width="43.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" customWidth="1"/>
-    <col min="8" max="9" width="33.109375" customWidth="1"/>
-    <col min="10" max="10" width="80.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="9.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2494,7 +2519,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>1</v>
       </c>
@@ -2525,7 +2550,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -2556,7 +2581,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -2579,7 +2604,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -2606,7 +2631,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>5</v>
       </c>
@@ -2635,7 +2660,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>6</v>
       </c>
@@ -2662,7 +2687,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>7</v>
       </c>
@@ -2689,7 +2714,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>8</v>
       </c>
@@ -2716,7 +2741,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -2741,18 +2766,43 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>655</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2765,6 +2815,7 @@
     <hyperlink ref="C9" location="Moodys_1909_Stock_Ratings!A1" display="Moodys_1909_Stock_Ratings"/>
     <hyperlink ref="C10" location="MonthlyNYSEStockPriceData!A1" display="MonthlyNYSEStockPriceData"/>
     <hyperlink ref="C11" location="Security_Characteristics_HP!A1" display="Security_Characteristics_HP_20140211"/>
+    <hyperlink ref="C12" location="city_state_list!A1" display="city_state_list"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2779,61 +2830,61 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>642</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>643</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -2844,89 +2895,189 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:C10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="MetaData!A1" display="back to meta data table of contents"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>656</v>
+      </c>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>42619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>655</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>654</v>
+      </c>
+      <c r="B13" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>657</v>
+      </c>
+      <c r="B14" t="s">
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -2948,61 +3099,61 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -3013,7 +3164,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -3021,7 +3172,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -3029,7 +3180,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -3037,7 +3188,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -3045,7 +3196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -3053,7 +3204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -3061,7 +3212,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -3069,7 +3220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -3077,7 +3228,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -3085,7 +3236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3093,7 +3244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -3101,7 +3252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -3109,7 +3260,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -3117,7 +3268,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -3125,7 +3276,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -3133,7 +3284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -3141,7 +3292,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -3149,7 +3300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -3157,7 +3308,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -3165,7 +3316,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -3173,7 +3324,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -3181,7 +3332,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>194</v>
       </c>
@@ -3189,7 +3340,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -3197,7 +3348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -3205,7 +3356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -3213,7 +3364,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>198</v>
       </c>
@@ -3221,7 +3372,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>199</v>
       </c>
@@ -3229,7 +3380,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>200</v>
       </c>
@@ -3237,7 +3388,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>201</v>
       </c>
@@ -3245,7 +3396,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>202</v>
       </c>
@@ -3253,7 +3404,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>203</v>
       </c>
@@ -3261,7 +3412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>204</v>
       </c>
@@ -3269,7 +3420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>205</v>
       </c>
@@ -3277,7 +3428,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -3285,7 +3436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -3293,7 +3444,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -3301,7 +3452,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -3309,7 +3460,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -3317,7 +3468,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>207</v>
       </c>
@@ -3325,7 +3476,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>208</v>
       </c>
@@ -3333,7 +3484,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>209</v>
       </c>
@@ -3341,7 +3492,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>210</v>
       </c>
@@ -3349,7 +3500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>211</v>
       </c>
@@ -3357,7 +3508,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>212</v>
       </c>
@@ -3365,7 +3516,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>213</v>
       </c>
@@ -3373,7 +3524,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>214</v>
       </c>
@@ -3381,7 +3532,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>215</v>
       </c>
@@ -3389,7 +3540,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>216</v>
       </c>
@@ -3397,7 +3548,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>217</v>
       </c>
@@ -3405,7 +3556,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>218</v>
       </c>
@@ -3413,7 +3564,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>219</v>
       </c>
@@ -3421,7 +3572,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>220</v>
       </c>
@@ -3429,7 +3580,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>221</v>
       </c>
@@ -3437,7 +3588,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>222</v>
       </c>
@@ -3445,7 +3596,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>223</v>
       </c>
@@ -3453,7 +3604,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>224</v>
       </c>
@@ -3461,7 +3612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>225</v>
       </c>
@@ -3469,7 +3620,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>226</v>
       </c>
@@ -3477,7 +3628,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>227</v>
       </c>
@@ -3485,7 +3636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>228</v>
       </c>
@@ -3493,7 +3644,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>229</v>
       </c>
@@ -3501,7 +3652,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>230</v>
       </c>
@@ -3509,7 +3660,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>231</v>
       </c>
@@ -3517,7 +3668,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>232</v>
       </c>
@@ -3525,7 +3676,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>233</v>
       </c>
@@ -3533,7 +3684,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>234</v>
       </c>
@@ -3541,7 +3692,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>235</v>
       </c>
@@ -3549,7 +3700,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>236</v>
       </c>
@@ -3557,7 +3708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>237</v>
       </c>
@@ -3565,7 +3716,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>238</v>
       </c>
@@ -3573,7 +3724,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>239</v>
       </c>
@@ -3581,7 +3732,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>240</v>
       </c>
@@ -3589,7 +3740,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -3597,7 +3748,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>242</v>
       </c>
@@ -3605,7 +3756,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>243</v>
       </c>
@@ -3613,7 +3764,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>244</v>
       </c>
@@ -3621,7 +3772,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>245</v>
       </c>
@@ -3629,7 +3780,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>246</v>
       </c>
@@ -3637,7 +3788,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>247</v>
       </c>
@@ -3645,7 +3796,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>248</v>
       </c>
@@ -3653,7 +3804,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>249</v>
       </c>
@@ -3661,7 +3812,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>250</v>
       </c>
@@ -3669,7 +3820,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>251</v>
       </c>
@@ -3677,7 +3828,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>252</v>
       </c>
@@ -3685,7 +3836,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>253</v>
       </c>
@@ -3693,7 +3844,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>254</v>
       </c>
@@ -3701,7 +3852,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>255</v>
       </c>
@@ -3709,7 +3860,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>256</v>
       </c>
@@ -3717,7 +3868,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>257</v>
       </c>
@@ -3725,7 +3876,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>258</v>
       </c>
@@ -3733,7 +3884,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>259</v>
       </c>
@@ -3741,7 +3892,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>260</v>
       </c>
@@ -3749,7 +3900,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>134</v>
       </c>
@@ -3757,7 +3908,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -3765,7 +3916,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>136</v>
       </c>
@@ -3773,7 +3924,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>261</v>
       </c>
@@ -3781,7 +3932,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>262</v>
       </c>
@@ -3789,7 +3940,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>263</v>
       </c>
@@ -3797,7 +3948,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>264</v>
       </c>
@@ -3805,7 +3956,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>265</v>
       </c>
@@ -3813,7 +3964,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>266</v>
       </c>
@@ -3821,7 +3972,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>267</v>
       </c>
@@ -3829,7 +3980,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>268</v>
       </c>
@@ -3837,7 +3988,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>269</v>
       </c>
@@ -3845,7 +3996,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>270</v>
       </c>
@@ -3853,7 +4004,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>271</v>
       </c>
@@ -3861,7 +4012,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>272</v>
       </c>
@@ -3869,7 +4020,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>273</v>
       </c>
@@ -3877,7 +4028,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>274</v>
       </c>
@@ -3885,7 +4036,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>275</v>
       </c>
@@ -3893,7 +4044,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>276</v>
       </c>
@@ -3901,7 +4052,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>277</v>
       </c>
@@ -3909,7 +4060,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>278</v>
       </c>
@@ -3917,7 +4068,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>279</v>
       </c>
@@ -3925,7 +4076,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>280</v>
       </c>
@@ -3933,7 +4084,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>281</v>
       </c>
@@ -3941,7 +4092,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>282</v>
       </c>
@@ -3949,7 +4100,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>283</v>
       </c>
@@ -3957,7 +4108,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>284</v>
       </c>
@@ -3965,7 +4116,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>285</v>
       </c>
@@ -3973,7 +4124,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>286</v>
       </c>
@@ -3981,7 +4132,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>287</v>
       </c>
@@ -3989,7 +4140,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>288</v>
       </c>
@@ -3997,7 +4148,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>289</v>
       </c>
@@ -4005,7 +4156,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>290</v>
       </c>
@@ -4013,7 +4164,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>291</v>
       </c>
@@ -4021,7 +4172,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>292</v>
       </c>
@@ -4029,7 +4180,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>293</v>
       </c>
@@ -4037,7 +4188,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>294</v>
       </c>
@@ -4045,7 +4196,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>295</v>
       </c>
@@ -4053,7 +4204,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>296</v>
       </c>
@@ -4061,7 +4212,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>297</v>
       </c>
@@ -4069,7 +4220,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>298</v>
       </c>
@@ -4077,7 +4228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -4085,7 +4236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>173</v>
       </c>
@@ -4111,61 +4262,61 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>489</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>490</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -4176,7 +4327,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>412</v>
       </c>
@@ -4184,7 +4335,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>413</v>
       </c>
@@ -4192,7 +4343,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>467</v>
       </c>
@@ -4200,7 +4351,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>468</v>
       </c>
@@ -4208,7 +4359,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>469</v>
       </c>
@@ -4216,7 +4367,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>470</v>
       </c>
@@ -4224,7 +4375,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>471</v>
       </c>
@@ -4232,7 +4383,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>472</v>
       </c>
@@ -4240,7 +4391,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>473</v>
       </c>
@@ -4248,7 +4399,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>474</v>
       </c>
@@ -4256,7 +4407,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>475</v>
       </c>
@@ -4264,7 +4415,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>476</v>
       </c>
@@ -4272,7 +4423,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>477</v>
       </c>
@@ -4299,61 +4450,61 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>491</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -4364,7 +4515,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4372,7 +4523,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>492</v>
       </c>
@@ -4380,7 +4531,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>493</v>
       </c>
@@ -4388,7 +4539,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>494</v>
       </c>
@@ -4396,7 +4547,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>495</v>
       </c>
@@ -4404,7 +4555,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>496</v>
       </c>
@@ -4412,7 +4563,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>497</v>
       </c>
@@ -4420,7 +4571,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>498</v>
       </c>
@@ -4428,7 +4579,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>499</v>
       </c>
@@ -4436,7 +4587,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>500</v>
       </c>
@@ -4444,7 +4595,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>501</v>
       </c>
@@ -4452,7 +4603,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>502</v>
       </c>
@@ -4460,7 +4611,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>503</v>
       </c>
@@ -4468,7 +4619,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>504</v>
       </c>
@@ -4476,7 +4627,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>505</v>
       </c>
@@ -4484,7 +4635,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>506</v>
       </c>
@@ -4492,7 +4643,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>507</v>
       </c>
@@ -4500,7 +4651,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>508</v>
       </c>
@@ -4508,7 +4659,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>509</v>
       </c>
@@ -4516,7 +4667,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>510</v>
       </c>
@@ -4524,7 +4675,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>511</v>
       </c>
@@ -4532,7 +4683,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>512</v>
       </c>
@@ -4540,7 +4691,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>513</v>
       </c>
@@ -4548,7 +4699,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>514</v>
       </c>
@@ -4556,7 +4707,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>515</v>
       </c>
@@ -4564,7 +4715,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>516</v>
       </c>
@@ -4572,7 +4723,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>517</v>
       </c>
@@ -4580,7 +4731,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>518</v>
       </c>
@@ -4588,7 +4739,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>519</v>
       </c>
@@ -4596,7 +4747,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>520</v>
       </c>
@@ -4604,7 +4755,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>521</v>
       </c>
@@ -4612,7 +4763,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>522</v>
       </c>
@@ -4620,7 +4771,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>523</v>
       </c>
@@ -4628,7 +4779,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>524</v>
       </c>
@@ -4636,7 +4787,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>525</v>
       </c>
@@ -4644,7 +4795,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>526</v>
       </c>
@@ -4652,7 +4803,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>527</v>
       </c>
@@ -4660,7 +4811,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>528</v>
       </c>
@@ -4668,7 +4819,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>529</v>
       </c>
@@ -4676,7 +4827,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>530</v>
       </c>
@@ -4684,7 +4835,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>531</v>
       </c>
@@ -4692,7 +4843,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>532</v>
       </c>
@@ -4700,7 +4851,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>533</v>
       </c>
@@ -4708,7 +4859,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>534</v>
       </c>
@@ -4716,7 +4867,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>535</v>
       </c>
@@ -4724,7 +4875,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>536</v>
       </c>
@@ -4732,7 +4883,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>537</v>
       </c>
@@ -4740,7 +4891,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>538</v>
       </c>
@@ -4748,7 +4899,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>539</v>
       </c>
@@ -4756,7 +4907,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>540</v>
       </c>
@@ -4764,7 +4915,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>541</v>
       </c>
@@ -4772,7 +4923,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>542</v>
       </c>
@@ -4780,7 +4931,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>543</v>
       </c>
@@ -4788,7 +4939,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>544</v>
       </c>
@@ -4796,7 +4947,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>545</v>
       </c>
@@ -4804,7 +4955,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>546</v>
       </c>
@@ -4812,7 +4963,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>547</v>
       </c>
@@ -4820,7 +4971,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>548</v>
       </c>
@@ -4828,7 +4979,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>549</v>
       </c>
@@ -4836,7 +4987,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>550</v>
       </c>
@@ -4844,7 +4995,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>551</v>
       </c>
@@ -4852,7 +5003,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>552</v>
       </c>
@@ -4860,7 +5011,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>553</v>
       </c>
@@ -4868,7 +5019,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>554</v>
       </c>
@@ -4876,7 +5027,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>555</v>
       </c>
@@ -4884,7 +5035,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>556</v>
       </c>
@@ -4892,7 +5043,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>557</v>
       </c>
@@ -4900,7 +5051,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -4908,7 +5059,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>559</v>
       </c>
@@ -4916,7 +5067,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>560</v>
       </c>
@@ -4924,7 +5075,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>561</v>
       </c>
@@ -4932,7 +5083,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>562</v>
       </c>
@@ -4940,7 +5091,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>563</v>
       </c>
@@ -4948,7 +5099,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>564</v>
       </c>
@@ -4956,7 +5107,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>565</v>
       </c>
@@ -4964,7 +5115,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>566</v>
       </c>
@@ -4989,61 +5140,61 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>651</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5054,7 +5205,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>412</v>
       </c>
@@ -5062,7 +5213,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>413</v>
       </c>
@@ -5070,7 +5221,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>414</v>
       </c>
@@ -5078,7 +5229,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>415</v>
       </c>
@@ -5086,7 +5237,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>318</v>
       </c>
@@ -5094,7 +5245,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>418</v>
       </c>
@@ -5102,7 +5253,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -5110,7 +5261,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>419</v>
       </c>
@@ -5118,7 +5269,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -5126,7 +5277,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>420</v>
       </c>
@@ -5134,7 +5285,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>421</v>
       </c>
@@ -5142,7 +5293,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>422</v>
       </c>
@@ -5150,7 +5301,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>423</v>
       </c>
@@ -5158,7 +5309,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>424</v>
       </c>
@@ -5166,7 +5317,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>425</v>
       </c>
@@ -5174,7 +5325,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>644</v>
       </c>
@@ -5182,7 +5333,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>645</v>
       </c>
@@ -5190,7 +5341,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>646</v>
       </c>
@@ -5198,7 +5349,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>312</v>
       </c>
@@ -5206,7 +5357,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>432</v>
       </c>
@@ -5214,7 +5365,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>647</v>
       </c>
@@ -5222,7 +5373,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>434</v>
       </c>
@@ -5230,7 +5381,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>435</v>
       </c>
@@ -5238,7 +5389,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>436</v>
       </c>
@@ -5246,7 +5397,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>437</v>
       </c>
@@ -5273,61 +5424,61 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>465</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>466</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5338,7 +5489,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>412</v>
       </c>
@@ -5346,7 +5497,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>413</v>
       </c>
@@ -5354,7 +5505,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>414</v>
       </c>
@@ -5362,7 +5513,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>415</v>
       </c>
@@ -5370,7 +5521,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>318</v>
       </c>
@@ -5378,7 +5529,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>416</v>
       </c>
@@ -5386,7 +5537,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>417</v>
       </c>
@@ -5394,7 +5545,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>418</v>
       </c>
@@ -5402,7 +5553,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -5410,7 +5561,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>419</v>
       </c>
@@ -5418,7 +5569,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -5426,7 +5577,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>420</v>
       </c>
@@ -5434,7 +5585,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>421</v>
       </c>
@@ -5442,7 +5593,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>422</v>
       </c>
@@ -5450,7 +5601,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>423</v>
       </c>
@@ -5458,7 +5609,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>424</v>
       </c>
@@ -5466,7 +5617,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>425</v>
       </c>
@@ -5474,7 +5625,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>426</v>
       </c>
@@ -5482,7 +5633,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>427</v>
       </c>
@@ -5490,7 +5641,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>428</v>
       </c>
@@ -5498,7 +5649,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>429</v>
       </c>
@@ -5506,7 +5657,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>430</v>
       </c>
@@ -5514,7 +5665,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>431</v>
       </c>
@@ -5522,7 +5673,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>312</v>
       </c>
@@ -5530,7 +5681,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>432</v>
       </c>
@@ -5538,7 +5689,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>433</v>
       </c>
@@ -5546,7 +5697,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>434</v>
       </c>
@@ -5554,7 +5705,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>435</v>
       </c>
@@ -5562,7 +5713,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>436</v>
       </c>
@@ -5570,7 +5721,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>437</v>
       </c>
@@ -5595,61 +5746,61 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>335</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5660,77 +5811,77 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -5752,61 +5903,61 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>346</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5817,72 +5968,72 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>356</v>
       </c>
@@ -5904,61 +6055,61 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>409</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>42585</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5969,7 +6120,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>384</v>
       </c>
@@ -5977,7 +6128,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>385</v>
       </c>
@@ -5985,7 +6136,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>386</v>
       </c>
@@ -5993,7 +6144,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>387</v>
       </c>
@@ -6001,7 +6152,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>388</v>
       </c>
@@ -6009,7 +6160,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>389</v>
       </c>
@@ -6017,7 +6168,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>390</v>
       </c>
@@ -6025,7 +6176,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>391</v>
       </c>
@@ -6033,7 +6184,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>392</v>
       </c>
@@ -6041,7 +6192,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>393</v>
       </c>
@@ -6049,7 +6200,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>394</v>
       </c>
@@ -6057,7 +6208,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>395</v>
       </c>
@@ -6065,7 +6216,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>396</v>
       </c>
@@ -6073,7 +6224,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>397</v>
       </c>
@@ -6081,7 +6232,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>398</v>
       </c>
@@ -6089,7 +6240,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>399</v>
       </c>
@@ -6097,7 +6248,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>400</v>
       </c>
@@ -6105,7 +6256,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>375</v>
       </c>
@@ -6113,7 +6264,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>401</v>
       </c>
@@ -6121,7 +6272,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>402</v>
       </c>
@@ -6129,7 +6280,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>403</v>
       </c>
@@ -6137,7 +6288,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>404</v>
       </c>
@@ -6145,7 +6296,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>405</v>
       </c>
@@ -6153,7 +6304,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>406</v>
       </c>
@@ -6161,7 +6312,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>407</v>
       </c>
@@ -6169,7 +6320,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>408</v>
       </c>

</xml_diff>